<commit_message>
All current card actions preliminarily entered
</commit_message>
<xml_diff>
--- a/public/res/Cards.xlsx
+++ b/public/res/Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lbcdn\Documents\Processing\shift\public\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851F70DD-E977-463B-A859-A9DE33F07D08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5A346D-971D-4EF6-9B0A-5E72FF359890}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="367" yWindow="367" windowWidth="19200" windowHeight="10213" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="117">
   <si>
     <t>Deck</t>
   </si>
@@ -102,9 +102,6 @@
     <t>virus</t>
   </si>
   <si>
-    <t xml:space="preserve">On play, lose two cards. You may choose to add this </t>
-  </si>
-  <si>
     <t>Power Outage!</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>Force Exit</t>
   </si>
   <si>
-    <t>You may move up to two program or virus cards between players</t>
-  </si>
-  <si>
     <t>Screen Sharing</t>
   </si>
   <si>
@@ -165,9 +159,6 @@
     <t>Networking</t>
   </si>
   <si>
-    <t>Gather all programs and virus, shuffle, redistribute equally</t>
-  </si>
-  <si>
     <t>December '69</t>
   </si>
   <si>
@@ -189,12 +180,6 @@
     <t>If you have Registry and Task Manager</t>
   </si>
   <si>
-    <t>Off, Then On</t>
-  </si>
-  <si>
-    <t>If you loose all cards in your hand then draw again</t>
-  </si>
-  <si>
     <t>A Millenial's Touch</t>
   </si>
   <si>
@@ -210,15 +195,9 @@
     <t>Befriend a Prince</t>
   </si>
   <si>
-    <t>If you have Bad Link! and Antivirus.exe or Browser</t>
-  </si>
-  <si>
     <t>Faster, Hotter, Better</t>
   </si>
   <si>
-    <t>If you have Overclocked, any program and GPU Accelerated is in play</t>
-  </si>
-  <si>
     <t>Upgrade</t>
   </si>
   <si>
@@ -285,9 +264,6 @@
     <t>Bytes and Pieces</t>
   </si>
   <si>
-    <t>Draw 8 cards, then give a card to each player from your hand</t>
-  </si>
-  <si>
     <t>Just a Nibble</t>
   </si>
   <si>
@@ -379,6 +355,30 @@
   </si>
   <si>
     <t>tick</t>
+  </si>
+  <si>
+    <t>On play, lose two cards. You may choose to add this to the hand of the player who's turn is next.</t>
+  </si>
+  <si>
+    <t>Transfer two program or virus cards between players</t>
+  </si>
+  <si>
+    <t>Gather all programs and viruses, shuffle, redistribute equally</t>
+  </si>
+  <si>
+    <t>Off, Then On Again</t>
+  </si>
+  <si>
+    <t>If you start the turn with cards, play them all, and draw back up to 5</t>
+  </si>
+  <si>
+    <t>If you have Bad Link! and one of Antivirus.exe or Browser</t>
+  </si>
+  <si>
+    <t>If you have Overclocked, GPU Accelerated, and any program</t>
+  </si>
+  <si>
+    <t>You may draw 4 cards, then give a card to each player from your hand</t>
   </si>
 </sst>
 </file>
@@ -1221,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1232,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1403,7 +1403,7 @@
         <v>23</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.5">
@@ -1414,13 +1414,13 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
         <v>23</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.5">
@@ -1431,13 +1431,13 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
@@ -1448,13 +1448,13 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.5">
@@ -1465,13 +1465,13 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
         <v>31</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>32</v>
-      </c>
-      <c r="G14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.5">
@@ -1482,13 +1482,13 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" t="s">
         <v>34</v>
-      </c>
-      <c r="E15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
@@ -1499,13 +1499,13 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" t="s">
         <v>36</v>
-      </c>
-      <c r="E16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.5">
@@ -1516,13 +1516,13 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" t="s">
         <v>38</v>
-      </c>
-      <c r="E17" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.5">
@@ -1533,13 +1533,13 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.5">
@@ -1550,13 +1550,13 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.5">
@@ -1567,13 +1567,13 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.5">
@@ -1584,13 +1584,13 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.5">
@@ -1601,13 +1601,13 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.5">
@@ -1618,13 +1618,13 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" t="s">
         <v>49</v>
-      </c>
-      <c r="G23" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.5">
@@ -1635,13 +1635,13 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G24" t="s">
-        <v>54</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.5">
@@ -1652,13 +1652,13 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G25" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.5">
@@ -1669,13 +1669,13 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G26" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.5">
@@ -1686,13 +1686,13 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G27" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.5">
@@ -1703,13 +1703,13 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G28" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.5">
@@ -1720,16 +1720,16 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E29" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F29">
         <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.5">
@@ -1740,13 +1740,13 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E30" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G30" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.5">
@@ -1757,13 +1757,13 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E31" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G31" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.5">
@@ -1774,13 +1774,13 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G32" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.5">
@@ -1791,13 +1791,13 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G33" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.5">
@@ -1808,13 +1808,13 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G34" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.5">
@@ -1825,13 +1825,13 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E35" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G35" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.5">
@@ -1842,13 +1842,13 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E36" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G36" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.5">
@@ -1859,13 +1859,13 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E37" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G37" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.5">
@@ -1876,13 +1876,13 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G38" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.5">
@@ -1893,13 +1893,13 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G39" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.5">
@@ -1910,13 +1910,13 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E40" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G40" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.5">
@@ -1927,13 +1927,13 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E41" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G41" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.5">
@@ -1944,13 +1944,13 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E42" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G42" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.5">
@@ -1961,13 +1961,13 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E43" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G43" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.5">
@@ -1978,13 +1978,13 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E44" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G44" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.5">
@@ -1995,13 +1995,13 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E45" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G45" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.5">
@@ -2012,13 +2012,13 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E46" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G46" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.5">
@@ -2029,13 +2029,13 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
-      </c>
-      <c r="G47" t="s">
-        <v>100</v>
+        <v>108</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.5">
@@ -2046,10 +2046,10 @@
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E48" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -2063,52 +2063,28 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E49" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F49">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A50" t="s">
-        <v>6</v>
-      </c>
       <c r="B50">
         <v>48</v>
       </c>
-      <c r="C50" t="s">
-        <v>101</v>
-      </c>
-      <c r="E50" t="s">
-        <v>116</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A51" t="s">
-        <v>6</v>
-      </c>
       <c r="B51">
         <v>49</v>
       </c>
-      <c r="C51" t="s">
-        <v>101</v>
-      </c>
-      <c r="E51" t="s">
-        <v>116</v>
-      </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B52">
         <v>50</v>
@@ -2116,7 +2092,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B53">
         <v>51</v>
@@ -2124,7 +2100,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B54">
         <v>52</v>
@@ -2132,7 +2108,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B55">
         <v>53</v>
@@ -2140,7 +2116,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B56">
         <v>54</v>
@@ -2148,7 +2124,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B57">
         <v>55</v>
@@ -2156,7 +2132,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B58">
         <v>56</v>
@@ -2164,7 +2140,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B59">
         <v>57</v>
@@ -2172,7 +2148,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B60">
         <v>58</v>
@@ -2180,7 +2156,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B61">
         <v>59</v>
@@ -2188,7 +2164,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B62">
         <v>60</v>
@@ -2196,7 +2172,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B63">
         <v>61</v>
@@ -2204,7 +2180,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B64">
         <v>62</v>
@@ -2212,7 +2188,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B65">
         <v>63</v>
@@ -2220,7 +2196,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B66">
         <v>64</v>
@@ -2228,7 +2204,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B67">
         <v>65</v>
@@ -2236,7 +2212,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A68" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B68">
         <v>66</v>
@@ -2244,7 +2220,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A69" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B69">
         <v>67</v>
@@ -2252,7 +2228,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A70" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B70">
         <v>68</v>
@@ -2260,7 +2236,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A71" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B71">
         <v>69</v>
@@ -2268,7 +2244,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A72" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B72">
         <v>70</v>
@@ -2276,7 +2252,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A73" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B73">
         <v>71</v>
@@ -2284,7 +2260,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B74">
         <v>72</v>
@@ -2292,7 +2268,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A75" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B75">
         <v>73</v>
@@ -2300,7 +2276,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A76" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B76">
         <v>74</v>
@@ -2308,7 +2284,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A77" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B77">
         <v>75</v>
@@ -2316,7 +2292,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B78">
         <v>76</v>
@@ -2324,7 +2300,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A79" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B79">
         <v>77</v>
@@ -2332,7 +2308,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A80" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B80">
         <v>78</v>
@@ -2340,7 +2316,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B81">
         <v>79</v>
@@ -2348,7 +2324,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A82" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B82">
         <v>80</v>
@@ -2356,7 +2332,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A83" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B83">
         <v>81</v>
@@ -2364,7 +2340,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A84" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B84">
         <v>82</v>
@@ -2372,7 +2348,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A85" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B85">
         <v>83</v>
@@ -2380,7 +2356,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A86" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B86">
         <v>84</v>
@@ -2388,7 +2364,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A87" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B87">
         <v>85</v>
@@ -2396,7 +2372,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A88" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B88">
         <v>86</v>
@@ -2404,7 +2380,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A89" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B89">
         <v>87</v>
@@ -2412,7 +2388,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A90" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B90">
         <v>88</v>
@@ -2420,7 +2396,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A91" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B91">
         <v>89</v>
@@ -2428,7 +2404,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A92" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B92">
         <v>90</v>
@@ -2436,7 +2412,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B93">
         <v>91</v>
@@ -2444,7 +2420,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A94" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B94">
         <v>92</v>
@@ -2452,7 +2428,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A95" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B95">
         <v>93</v>
@@ -2460,7 +2436,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A96" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B96">
         <v>94</v>
@@ -2468,7 +2444,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A97" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B97">
         <v>95</v>
@@ -2476,7 +2452,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A98" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B98">
         <v>96</v>
@@ -2484,7 +2460,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B99">
         <v>97</v>
@@ -2492,7 +2468,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B100">
         <v>98</v>
@@ -2500,7 +2476,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B101">
         <v>99</v>
@@ -2508,7 +2484,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B102">
         <v>100</v>
@@ -2516,7 +2492,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A103" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B103">
         <v>101</v>
@@ -2524,7 +2500,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B104">
         <v>102</v>
@@ -2532,7 +2508,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B105">
         <v>103</v>
@@ -2540,7 +2516,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A106" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B106">
         <v>104</v>
@@ -2548,7 +2524,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A107" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B107">
         <v>105</v>
@@ -2556,7 +2532,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A108" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B108">
         <v>106</v>
@@ -2564,7 +2540,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A109" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B109">
         <v>107</v>
@@ -2572,7 +2548,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A110" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B110">
         <v>108</v>
@@ -2580,7 +2556,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A111" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B111">
         <v>109</v>
@@ -2588,7 +2564,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A112" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B112">
         <v>110</v>
@@ -2596,7 +2572,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A113" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B113">
         <v>111</v>
@@ -2604,7 +2580,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A114" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B114">
         <v>112</v>
@@ -2612,7 +2588,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A115" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B115">
         <v>113</v>
@@ -2620,7 +2596,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A116" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B116">
         <v>114</v>
@@ -2628,7 +2604,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A117" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B117">
         <v>115</v>
@@ -2636,7 +2612,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A118" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B118">
         <v>116</v>
@@ -2644,7 +2620,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A119" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B119">
         <v>117</v>
@@ -2652,7 +2628,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A120" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B120">
         <v>118</v>
@@ -2660,7 +2636,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A121" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B121">
         <v>119</v>
@@ -2668,7 +2644,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A122" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B122">
         <v>120</v>
@@ -2676,7 +2652,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A123" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B123">
         <v>121</v>
@@ -2684,7 +2660,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A124" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B124">
         <v>122</v>
@@ -2692,7 +2668,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A125" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B125">
         <v>123</v>
@@ -2700,7 +2676,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A126" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B126">
         <v>124</v>
@@ -2708,7 +2684,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A127" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B127">
         <v>125</v>
@@ -2716,7 +2692,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A128" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B128">
         <v>126</v>
@@ -2724,7 +2700,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A129" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B129">
         <v>127</v>
@@ -2732,7 +2708,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A130" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B130">
         <v>128</v>
@@ -2740,7 +2716,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A131" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B131">
         <v>129</v>
@@ -2748,7 +2724,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A132" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B132">
         <v>130</v>
@@ -2756,7 +2732,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A133" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B133">
         <v>131</v>
@@ -2764,7 +2740,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A134" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B134">
         <v>132</v>
@@ -2772,7 +2748,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A135" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B135">
         <v>133</v>
@@ -2780,7 +2756,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A136" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B136">
         <v>134</v>
@@ -2788,7 +2764,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A137" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B137">
         <v>135</v>
@@ -2796,7 +2772,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A138" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B138">
         <v>136</v>
@@ -2804,7 +2780,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A139" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B139">
         <v>137</v>
@@ -2812,7 +2788,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A140" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B140">
         <v>138</v>
@@ -2820,7 +2796,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A141" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B141">
         <v>139</v>
@@ -2828,7 +2804,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A142" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B142">
         <v>140</v>
@@ -2836,7 +2812,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A143" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B143">
         <v>141</v>
@@ -2844,7 +2820,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A144" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B144">
         <v>142</v>
@@ -2852,7 +2828,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A145" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B145">
         <v>143</v>
@@ -2860,7 +2836,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A146" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B146">
         <v>144</v>
@@ -2868,7 +2844,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A147" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B147">
         <v>145</v>
@@ -2876,7 +2852,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A148" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B148">
         <v>146</v>
@@ -2884,7 +2860,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A149" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B149">
         <v>147</v>
@@ -2892,7 +2868,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A150" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B150">
         <v>148</v>
@@ -2900,7 +2876,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A151" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B151">
         <v>149</v>
@@ -2913,96 +2889,116 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A6" sqref="A6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" t="s">
-        <v>111</v>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 D4:D5" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2 E4:E5" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"play, draw, command, end, time, script, program, virus"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>